<commit_message>
The PCB circuit of minifoc is modified
</commit_message>
<xml_diff>
--- a/manufacture/miniFOC/BOM_miniFOC.xlsx
+++ b/manufacture/miniFOC/BOM_miniFOC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Files\miniFOC\manufacture\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Files\miniFOC\manufacture\miniFOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3380BFE3-D7E6-4D75-8367-6BB646C1597C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB3C49A-10C0-44F0-B435-D821A731C4B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9012" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="73">
   <si>
     <t>100nF</t>
   </si>
@@ -61,9 +61,6 @@
     <t>GH1.25</t>
   </si>
   <si>
-    <t>J1,J2</t>
-  </si>
-  <si>
     <t>C225129</t>
   </si>
   <si>
@@ -79,12 +76,6 @@
     <t>4.7uH</t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>C32684</t>
-  </si>
-  <si>
     <t>AP2300</t>
   </si>
   <si>
@@ -202,10 +193,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>SMD_L6.0-W6.0</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>立创编号</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -246,6 +233,34 @@
   </si>
   <si>
     <t>C72041</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>C251690</t>
+  </si>
+  <si>
+    <t>SMD_L4.4-W4.0</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>C2829252</t>
+  </si>
+  <si>
+    <t>J2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GH1.25</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>GH1.25_3P_卧贴</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1218,10 +1233,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1236,22 +1251,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1296,7 +1311,7 @@
     </row>
     <row r="4" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
@@ -1322,7 +1337,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
@@ -1336,19 +1351,19 @@
     </row>
     <row r="6" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="1">
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1">
         <v>1.0497000000000001</v>
@@ -1356,19 +1371,19 @@
     </row>
     <row r="7" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="1">
         <v>3.88</v>
@@ -1376,39 +1391,39 @@
     </row>
     <row r="8" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1">
-        <v>0.4294</v>
+        <v>1.9060999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1">
         <v>6</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F9" s="1">
         <v>0.14410000000000001</v>
@@ -1416,19 +1431,19 @@
     </row>
     <row r="10" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F10" s="1">
         <v>7.3000000000000001E-3</v>
@@ -1436,19 +1451,19 @@
     </row>
     <row r="11" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1">
         <v>7.1999999999999998E-3</v>
@@ -1456,19 +1471,19 @@
     </row>
     <row r="12" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1">
         <v>8.0000000000000002E-3</v>
@@ -1476,19 +1491,19 @@
     </row>
     <row r="13" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1">
         <v>5.0599999999999999E-2</v>
@@ -1496,19 +1511,19 @@
     </row>
     <row r="14" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1">
         <v>5.01</v>
@@ -1516,19 +1531,19 @@
     </row>
     <row r="15" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1">
         <v>1.95</v>
@@ -1536,19 +1551,19 @@
     </row>
     <row r="16" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F16" s="1">
         <v>0.16539999999999999</v>
@@ -1556,19 +1571,19 @@
     </row>
     <row r="17" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1">
         <v>0.66539999999999999</v>
@@ -1576,22 +1591,42 @@
     </row>
     <row r="18" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D18" s="2">
         <v>1</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F18" s="1">
         <v>9.8599999999999993E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.3221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>